<commit_message>
Improved database for Norway and Italy, added storage check in postprocessing
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigEU.xlsx
+++ b/ConfigFiles/ConfigEU.xlsx
@@ -969,15 +969,15 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
@@ -1851,7 +1851,7 @@
         <v>27</v>
       </c>
       <c r="F101" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Outages added to the database, ConfigEU file updated to include outages and new profiles
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigEU.xlsx
+++ b/ConfigFiles/ConfigEU.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="156">
   <si>
     <t>Default value</t>
   </si>
@@ -474,13 +474,16 @@
     <t>Clustered simulation for EU. Small or highly flexible units are clustered.</t>
   </si>
   <si>
-    <t>Database/HydroData/ScaledInflows/##/1h/2016_converted_from_2012.csv</t>
-  </si>
-  <si>
     <t>Simulations/simulationEUshort</t>
   </si>
   <si>
     <t>Database/HydroData/ScaledLevels/##/1h/2016.csv</t>
+  </si>
+  <si>
+    <t>Database/OutageFactors/##/2016.csv</t>
+  </si>
+  <si>
+    <t>Database/HydroData/ScaledInflows/##/1h/2016_profile_from_2012.csv</t>
   </si>
 </sst>
 </file>
@@ -970,7 +973,7 @@
   <dimension ref="A1:H165"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1077,7 @@
         <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18" s="14"/>
       <c r="H18" s="1" t="s">
@@ -1178,7 +1181,7 @@
         <v>39</v>
       </c>
       <c r="C32" s="21">
-        <v>42735</v>
+        <v>42376</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>75</v>
@@ -1307,7 +1310,9 @@
       <c r="B63" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C63" s="28"/>
+      <c r="C63" s="28" t="s">
+        <v>154</v>
+      </c>
       <c r="D63" s="22" t="s">
         <v>92</v>
       </c>
@@ -1409,7 +1414,7 @@
         <v>37</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D69" s="22" t="s">
         <v>92</v>
@@ -1535,7 +1540,7 @@
         <v>37</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D76" s="22" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Update to ConfigEU to include heat demand for BIO units
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigEU.xlsx
+++ b/ConfigFiles/ConfigEU.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\Dispa-SET-MidTermScheduling\Dispa_EU\ConfigFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C637D195-29F7-4CFF-8DB5-67241D169F81}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="1185"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="157">
   <si>
     <t>Default value</t>
   </si>
@@ -459,37 +465,40 @@
     <t>Database/TotalLoadValue/##/1h/2016.csv</t>
   </si>
   <si>
+    <t>Database/AvailabilityFactors/##/1h/2016.csv</t>
+  </si>
+  <si>
+    <t>Database/DayAheadNTC/1h/2016.csv</t>
+  </si>
+  <si>
+    <t>Database/CrossBorderFlows/1h/2016.csv</t>
+  </si>
+  <si>
+    <t>Clustered simulation for EU. Small or highly flexible units are clustered.</t>
+  </si>
+  <si>
+    <t>Database/HydroData/ScaledLevels/##/1h/2016.csv</t>
+  </si>
+  <si>
+    <t>Database/HydroData/ScaledInflows/##/1h/2016_profile_from_2012.csv</t>
+  </si>
+  <si>
+    <t>Database/OutageFactors/##/2016.csv</t>
+  </si>
+  <si>
     <t>Database/PowerPlants/##/clustered.csv</t>
   </si>
   <si>
-    <t>Database/AvailabilityFactors/##/1h/2016.csv</t>
-  </si>
-  <si>
-    <t>Database/DayAheadNTC/1h/2016.csv</t>
-  </si>
-  <si>
-    <t>Database/CrossBorderFlows/1h/2016.csv</t>
-  </si>
-  <si>
-    <t>Clustered simulation for EU. Small or highly flexible units are clustered.</t>
+    <t>Database/Heat_demand/##/Heat_Demand.csv</t>
   </si>
   <si>
     <t>Simulations/simulationEUshort</t>
-  </si>
-  <si>
-    <t>Database/HydroData/ScaledLevels/##/1h/2016.csv</t>
-  </si>
-  <si>
-    <t>Database/OutageFactors/##/2016.csv</t>
-  </si>
-  <si>
-    <t>Database/HydroData/ScaledInflows/##/1h/2016_profile_from_2012.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -572,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -587,9 +596,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -607,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -615,12 +621,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -635,11 +635,8 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -650,7 +647,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -659,14 +656,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,6 +671,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -725,7 +722,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -758,9 +755,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -793,6 +807,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -968,40 +999,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="20.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="96.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+    </row>
+    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1011,65 +1042,65 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="32" t="s">
+    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-    </row>
-    <row r="5" spans="1:8" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-    </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+    </row>
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-    </row>
-    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-    </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="C8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
@@ -1077,14 +1108,14 @@
         <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D18" s="14"/>
+        <v>156</v>
+      </c>
+      <c r="D18" s="13"/>
       <c r="H18" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -1098,7 +1129,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -1112,7 +1143,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
@@ -1126,7 +1157,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>88</v>
       </c>
@@ -1137,7 +1168,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>135</v>
       </c>
@@ -1145,49 +1176,49 @@
         <v>89</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:8" ht="0.75" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="C30" s="17"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="21">
+      <c r="C31" s="18">
         <v>42370</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="18">
         <v>42376</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>47</v>
       </c>
@@ -1201,7 +1232,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>49</v>
       </c>
@@ -1212,23 +1243,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="C45" s="17"/>
-    </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:8" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
+      <c r="C45" s="14"/>
+    </row>
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>43</v>
       </c>
@@ -1242,7 +1273,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>63</v>
       </c>
@@ -1256,7 +1287,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>129</v>
       </c>
@@ -1270,96 +1301,96 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:8" s="11" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="10"/>
-      <c r="C60" s="18"/>
-    </row>
-    <row r="61" spans="1:8" s="9" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
-      <c r="C61" s="17"/>
-    </row>
-    <row r="62" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
+    <row r="50" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:8" s="10" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="9"/>
+      <c r="C60" s="15"/>
+    </row>
+    <row r="61" spans="1:8" s="8" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="7"/>
+      <c r="C61" s="14"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="B62" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C62" s="23" t="s">
+      <c r="C62" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="D62" s="22" t="s">
+      <c r="D62" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="H62" s="12"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H62" s="11"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C63" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="D63" s="22" t="s">
+      <c r="C63" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D63" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="H63" s="12" t="s">
+      <c r="H63" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C64" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="D64" s="22" t="s">
+      <c r="C64" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="D64" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="H64" s="12" t="s">
+      <c r="H64" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C65" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D65" s="22" t="s">
+      <c r="C65" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D65" s="19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C66" s="24"/>
-      <c r="D66" s="22" t="s">
+      <c r="C66" s="20"/>
+      <c r="D66" s="19" t="s">
         <v>92</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -1368,70 +1399,70 @@
       <c r="F66" s="5">
         <v>0.05</v>
       </c>
-      <c r="H66" s="12" t="s">
+      <c r="H66" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C67" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="D67" s="22" t="s">
+      <c r="C67" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D67" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="H67" s="12" t="s">
+      <c r="H67" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C68" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="D68" s="22" t="s">
+      <c r="C68" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D68" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="H68" s="12" t="s">
+      <c r="H68" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C69" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="D69" s="22" t="s">
+      <c r="C69" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="D69" s="19" t="s">
         <v>92</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C70" s="24"/>
-      <c r="D70" s="22"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="19"/>
       <c r="E70" s="1" t="s">
         <v>0</v>
       </c>
@@ -1439,15 +1470,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C71" s="24"/>
-      <c r="D71" s="22" t="s">
+      <c r="C71" s="20"/>
+      <c r="D71" s="19" t="s">
         <v>92</v>
       </c>
       <c r="E71" s="1" t="s">
@@ -1457,15 +1488,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C72" s="24"/>
-      <c r="D72" s="22" t="s">
+      <c r="C72" s="20"/>
+      <c r="D72" s="19" t="s">
         <v>92</v>
       </c>
       <c r="E72" s="1" t="s">
@@ -1478,15 +1509,15 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C73" s="24"/>
-      <c r="D73" s="22" t="s">
+      <c r="C73" s="20"/>
+      <c r="D73" s="19" t="s">
         <v>92</v>
       </c>
       <c r="E73" s="1" t="s">
@@ -1496,33 +1527,33 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C74" s="24"/>
-      <c r="D74" s="22" t="s">
+      <c r="C74" s="20"/>
+      <c r="D74" s="19" t="s">
         <v>92</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F74" s="5">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C75" s="24"/>
-      <c r="D75" s="22" t="s">
+      <c r="C75" s="20"/>
+      <c r="D75" s="19" t="s">
         <v>92</v>
       </c>
       <c r="E75" s="1" t="s">
@@ -1532,29 +1563,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="D76" s="22" t="s">
+      <c r="C76" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D76" s="19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C77" s="24"/>
-      <c r="D77" s="22" t="s">
+      <c r="C77" s="20"/>
+      <c r="D77" s="19" t="s">
         <v>92</v>
       </c>
       <c r="E77" s="1" t="s">
@@ -1564,15 +1595,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C78" s="24"/>
-      <c r="D78" s="22" t="s">
+      <c r="C78" s="20"/>
+      <c r="D78" s="19" t="s">
         <v>92</v>
       </c>
       <c r="E78" s="1" t="s">
@@ -1582,27 +1613,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C79" s="24"/>
-      <c r="D79" s="22" t="s">
+      <c r="C79" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D79" s="19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C80" s="24"/>
-      <c r="D80" s="22" t="s">
+      <c r="C80" s="20"/>
+      <c r="D80" s="19" t="s">
         <v>92</v>
       </c>
       <c r="E80" s="1" t="s">
@@ -1612,15 +1645,15 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C81" s="24"/>
-      <c r="D81" s="22" t="s">
+      <c r="C81" s="20"/>
+      <c r="D81" s="19" t="s">
         <v>92</v>
       </c>
       <c r="E81" s="1" t="s">
@@ -1630,31 +1663,30 @@
         <v>400</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:8" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:8" s="11" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="10"/>
-      <c r="C85" s="18"/>
-    </row>
-    <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="1:8" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="1:8" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="9"/>
+      <c r="C85" s="15"/>
+    </row>
+    <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B87" s="6"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="30" t="s">
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B88" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C88" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E88" s="7" t="s">
+      <c r="E88" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F88" s="5" t="b">
@@ -1664,210 +1696,210 @@
         <v>144</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="30"/>
-      <c r="B89" s="7" t="s">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89" s="26"/>
+      <c r="B89" s="6" t="s">
         <v>138</v>
       </c>
       <c r="C89" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E89" s="7" t="s">
+      <c r="E89" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F89" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="30"/>
-      <c r="B90" s="7" t="s">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90" s="26"/>
+      <c r="B90" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C90" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E90" s="7" t="s">
+      <c r="E90" s="6" t="s">
         <v>18</v>
       </c>
       <c r="F90" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="30"/>
-      <c r="B91" s="7" t="s">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A91" s="26"/>
+      <c r="B91" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C91" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E91" s="7" t="s">
+      <c r="E91" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F91" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="30"/>
-      <c r="B92" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92" s="26"/>
+      <c r="B92" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C92" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E92" s="7" t="s">
+      <c r="E92" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F92" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="30"/>
-      <c r="B93" s="7" t="s">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93" s="26"/>
+      <c r="B93" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C93" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E93" s="7" t="s">
+      <c r="E93" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F93" s="5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="30"/>
-      <c r="B94" s="7" t="s">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A94" s="26"/>
+      <c r="B94" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C94" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E94" s="7" t="s">
+      <c r="E94" s="6" t="s">
         <v>139</v>
       </c>
       <c r="F94" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
-      <c r="B95" s="7" t="s">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A95" s="26"/>
+      <c r="B95" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C95" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E95" s="7" t="s">
+      <c r="E95" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F95" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="30"/>
-      <c r="B96" s="7" t="s">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96" s="26"/>
+      <c r="B96" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C96" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E96" s="7" t="s">
+      <c r="E96" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F96" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="30"/>
-      <c r="B97" s="7" t="s">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A97" s="26"/>
+      <c r="B97" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C97" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E97" s="7" t="s">
+      <c r="E97" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F97" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="30"/>
-      <c r="B98" s="7" t="s">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A98" s="26"/>
+      <c r="B98" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C98" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E98" s="7" t="s">
+      <c r="E98" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F98" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="30"/>
-      <c r="B99" s="7" t="s">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99" s="26"/>
+      <c r="B99" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C99" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E99" s="7" t="s">
+      <c r="E99" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F99" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="30"/>
-      <c r="B100" s="7" t="s">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A100" s="26"/>
+      <c r="B100" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C100" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E100" s="7" t="s">
+      <c r="E100" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F100" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="30"/>
-      <c r="B101" s="7" t="s">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" s="26"/>
+      <c r="B101" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C101" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E101" s="7" t="s">
+      <c r="E101" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F101" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="30"/>
-      <c r="B102" s="7" t="s">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="26"/>
+      <c r="B102" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C102" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E102" s="7" t="s">
+      <c r="E102" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F102" s="5" t="b">
@@ -1877,23 +1909,23 @@
         <v>145</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="10"/>
-      <c r="C109" s="18"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="9"/>
+      <c r="C109" s="15"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="15" t="s">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -1903,7 +1935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>77</v>
       </c>
@@ -1917,7 +1949,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>78</v>
       </c>
@@ -1931,7 +1963,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>80</v>
       </c>
@@ -1942,148 +1974,148 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="10"/>
-      <c r="C128" s="18"/>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="128" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="9"/>
+      <c r="C128" s="15"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B132" s="27" t="s">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B132" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="C132" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B133" s="27" t="s">
+      <c r="C132" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B133" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C133" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B134" s="27" t="s">
+      <c r="C133" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B134" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C134" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B135" s="27" t="s">
+      <c r="C134" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B135" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C135" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B136" s="27" t="s">
+      <c r="C135" s="22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B136" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C136" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B137" s="27" t="s">
+      <c r="C136" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B137" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C137" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B138" s="27" t="s">
+      <c r="C137" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B138" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C138" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B139" s="27" t="s">
+      <c r="C138" s="22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B139" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="C139" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B140" s="27" t="s">
+      <c r="C139" s="22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B140" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C140" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B141" s="27" t="s">
+      <c r="C140" s="22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B141" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C141" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B142" s="27" t="s">
+      <c r="C141" s="22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B142" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C142" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B143" s="27" t="s">
+      <c r="C142" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B143" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C143" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="27" t="s">
+      <c r="C143" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B144" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C144" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B145" s="27" t="s">
+      <c r="C144" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B145" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C145" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B146" s="27" t="s">
+      <c r="C145" s="22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B146" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="C146" s="26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="C146" s="22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F165" s="2"/>
     </row>
   </sheetData>
@@ -2094,32 +2126,32 @@
     <mergeCell ref="B4:H4"/>
   </mergeCells>
   <dataValidations count="17">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C18:D18"/>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C31">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C18:D18" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
       <formula2>73051</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Stop day of the simulation" prompt="This is the last simulated day. It must be comprised within the range of dates provided within the data files." sqref="C32">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Stop day of the simulation" prompt="This is the last simulated day. It must be comprised within the range of dates provided within the data files." sqref="C32" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>1</formula1>
       <formula2>73051</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Historical interconnection flows" prompt="Historical flows" sqref="C68"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F70:F74 F77:F78 F80:F81"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C112"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C113"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C114"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C115"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C22"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F66"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F75"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C23"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reservoir inflows in MWh" sqref="C69"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C63"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Look Ahead Period" prompt="This is the overlap period between consecutive optimization of the rolling horizon._x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C34">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Historical interconnection flows" prompt="Historical flows" sqref="C68" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F70:F74 F77:F78 F80:F81" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C112" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C113" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C114" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C115" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C22" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F66" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F75" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C23" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reservoir inflows in MWh" sqref="C69" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C63" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Look Ahead Period" prompt="This is the overlap period between consecutive optimization of the rolling horizon._x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C34" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>0</formula1>
       <formula2>365</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Horizon length" prompt="This is the number of days to be optimized in the rolling horizon framework. Does not include the overlap period with the next optimization horizon. _x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C33">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Horizon length" prompt="This is the number of days to be optimized in the rolling horizon framework. Does not include the overlap period with the next optimization horizon. _x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C33" xr:uid="{00000000-0002-0000-0000-000010000000}">
       <formula1>1</formula1>
       <formula2>365</formula2>
     </dataValidation>
@@ -2129,43 +2161,43 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000011000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>F88:G102 C88:C102 C132:C146</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write excel files" prompt="If set to true, one excel file per parameter will be written in the simulation environment directory.">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write excel files" prompt="If set to true, one excel file per parameter will be written in the simulation environment directory." xr:uid="{00000000-0002-0000-0000-000012000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>C19:D19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write GDX file" prompt="If set to true, the gdx file is written in the simulation environment directory. Note that the gdx file is required to run the GAMS optimization.">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write GDX file" prompt="If set to true, the gdx file is written in the simulation environment directory. Note that the gdx file is required to run the GAMS optimization." xr:uid="{00000000-0002-0000-0000-000013000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>C20:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write Pickles file" prompt="If set to true, one pickle file (python data format) is written in the simulation environment directory to allow quickly retrieving the simulation inputs">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write Pickles file" prompt="If set to true, one pickle file (python data format) is written in the simulation environment directory to allow quickly retrieving the simulation inputs" xr:uid="{00000000-0002-0000-0000-000014000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>C21:D21 D46</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve Calculation" prompt="This inputs allows selecting the metodology for reserve sizing_x000a_">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve Calculation" prompt="This inputs allows selecting the metodology for reserve sizing_x000a_" xr:uid="{00000000-0002-0000-0000-000015000000}">
           <x14:formula1>
             <xm:f>Lists!$C$2:$C$11</xm:f>
           </x14:formula1>
           <xm:sqref>C48</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Allow Curtailment of Renewables" prompt="Set to true to allow curtailment">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Allow Curtailment of Renewables" prompt="Set to true to allow curtailment" xr:uid="{00000000-0002-0000-0000-000016000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>C49</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Simulation type" prompt="Select the type of optimization to perform.">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Simulation type" prompt="Select the type of optimization to perform." xr:uid="{00000000-0002-0000-0000-000017000000}">
           <x14:formula1>
             <xm:f>Lists!$B$2:$B$6</xm:f>
           </x14:formula1>
@@ -2178,7 +2210,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -2186,29 +2218,29 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>44</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2222,7 +2254,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2233,7 +2265,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>46</v>
       </c>
@@ -2241,7 +2273,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>137</v>
       </c>
@@ -2249,7 +2281,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>140</v>
       </c>
@@ -2261,7 +2293,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O16"/>
   <sheetViews>
@@ -2269,769 +2301,769 @@
       <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="20"/>
+    <col min="1" max="1" width="9.109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="N2" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="O2" s="25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="B2" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" s="25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="B3" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" s="25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="B4" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" s="25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="B5" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="O6" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="B6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="N7" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" s="25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="B7" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M8" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="N8" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="O8" s="25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="B8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="O9" s="25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="B9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" s="25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="B10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M11" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="O11" s="25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="B11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="B12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="L13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="M13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="O13" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="B13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="L14" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="M14" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="N14" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="O14" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="B14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="O15" s="25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="B15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M16" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="O16" s="25" t="b">
+      <c r="B16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" s="21" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="D1:D30">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D1:D30">
     <sortCondition ref="D1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
all heat demands in a single file. Updated heat data checks for the clustered formulation
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigEU.xlsx
+++ b/ConfigFiles/ConfigEU.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\EnergyModellingTool\Dispa-SET-MidTermScheduling\Dispa_EU\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\svn\Dispa-SET_Public\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C637D195-29F7-4CFF-8DB5-67241D169F81}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2521CA-973D-4047-AA3B-CA4992C5357F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -474,9 +474,6 @@
     <t>Database/CrossBorderFlows/1h/2016.csv</t>
   </si>
   <si>
-    <t>Clustered simulation for EU. Small or highly flexible units are clustered.</t>
-  </si>
-  <si>
     <t>Database/HydroData/ScaledLevels/##/1h/2016.csv</t>
   </si>
   <si>
@@ -489,10 +486,13 @@
     <t>Database/PowerPlants/##/clustered.csv</t>
   </si>
   <si>
-    <t>Database/Heat_demand/##/Heat_Demand.csv</t>
-  </si>
-  <si>
-    <t>Simulations/simulationEUshort</t>
+    <t>Simulations/simulationEU</t>
+  </si>
+  <si>
+    <t>Clustered simulation for EU28 + Switzerland and Norway using 2016 data.</t>
+  </si>
+  <si>
+    <t>Database/Heat_demand/2016.csv</t>
   </si>
 </sst>
 </file>
@@ -1003,24 +1003,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="96.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="20.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>54</v>
       </c>
@@ -1032,7 +1032,7 @@
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
     </row>
-    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1042,8 +1042,8 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
         <v>59</v>
       </c>
@@ -1054,7 +1054,7 @@
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -1064,12 +1064,12 @@
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -1078,7 +1078,7 @@
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
     </row>
-    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1087,20 +1087,20 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
@@ -1108,14 +1108,14 @@
         <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D18" s="13"/>
       <c r="H18" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>88</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>135</v>
       </c>
@@ -1180,17 +1180,17 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="C30" s="14"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
@@ -1212,13 +1212,13 @@
         <v>39</v>
       </c>
       <c r="C32" s="18">
-        <v>42376</v>
+        <v>42735</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>47</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>49</v>
       </c>
@@ -1243,23 +1243,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:8" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:8" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="C45" s="14"/>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>43</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>63</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>129</v>
       </c>
@@ -1301,25 +1301,25 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:8" s="10" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:8" s="10" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
       <c r="C60" s="15"/>
     </row>
-    <row r="61" spans="1:8" s="8" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" s="8" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="C61" s="14"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="H62" s="11"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>1</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>37</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>92</v>
@@ -1351,7 +1351,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>37</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D64" s="19" t="s">
         <v>92</v>
@@ -1368,7 +1368,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>38</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>42</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>50</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>93</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>132</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>37</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D69" s="19" t="s">
         <v>92</v>
@@ -1454,7 +1454,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>125</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>94</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>64</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>65</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>126</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>127</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>130</v>
       </c>
@@ -1571,13 +1571,13 @@
         <v>37</v>
       </c>
       <c r="C76" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D76" s="19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>133</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>134</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>136</v>
       </c>
@@ -1621,13 +1621,13 @@
         <v>37</v>
       </c>
       <c r="C79" s="20" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D79" s="19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>142</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>143</v>
       </c>
@@ -1663,20 +1663,20 @@
         <v>400</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" spans="1:8" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" spans="1:8" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:8" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:8" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="9"/>
       <c r="C85" s="15"/>
     </row>
-    <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="26" t="s">
         <v>53</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="26"/>
       <c r="B89" s="6" t="s">
         <v>138</v>
@@ -1711,7 +1711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="26"/>
       <c r="B90" s="6" t="s">
         <v>5</v>
@@ -1726,7 +1726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="26"/>
       <c r="B91" s="6" t="s">
         <v>31</v>
@@ -1741,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="26"/>
       <c r="B92" s="6" t="s">
         <v>16</v>
@@ -1756,7 +1756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="26"/>
       <c r="B93" s="6" t="s">
         <v>6</v>
@@ -1771,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="26"/>
       <c r="B94" s="6" t="s">
         <v>8</v>
@@ -1786,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="26"/>
       <c r="B95" s="6" t="s">
         <v>7</v>
@@ -1801,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="26"/>
       <c r="B96" s="6" t="s">
         <v>9</v>
@@ -1816,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="26"/>
       <c r="B97" s="6" t="s">
         <v>11</v>
@@ -1831,7 +1831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="26"/>
       <c r="B98" s="6" t="s">
         <v>12</v>
@@ -1846,7 +1846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="26"/>
       <c r="B99" s="6" t="s">
         <v>28</v>
@@ -1861,7 +1861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="26"/>
       <c r="B100" s="6" t="s">
         <v>13</v>
@@ -1876,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="26"/>
       <c r="B101" s="6" t="s">
         <v>14</v>
@@ -1891,7 +1891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="26"/>
       <c r="B102" s="6" t="s">
         <v>20</v>
@@ -1909,22 +1909,22 @@
         <v>145</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="105" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="108" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="9"/>
       <c r="C109" s="15"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>2</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>77</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>78</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>80</v>
       </c>
@@ -1974,28 +1974,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="128" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="9"/>
       <c r="C128" s="15"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B132" s="23" t="s">
         <v>95</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B133" s="23" t="s">
         <v>96</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B134" s="23" t="s">
         <v>97</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B135" s="23" t="s">
         <v>98</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B136" s="23" t="s">
         <v>99</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B137" s="23" t="s">
         <v>100</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B138" s="23" t="s">
         <v>101</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B139" s="23" t="s">
         <v>102</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B140" s="23" t="s">
         <v>103</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B141" s="23" t="s">
         <v>104</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B142" s="23" t="s">
         <v>105</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B143" s="23" t="s">
         <v>106</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" s="23" t="s">
         <v>107</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="23" t="s">
         <v>108</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" s="23" t="s">
         <v>109</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F165" s="2"/>
     </row>
   </sheetData>
@@ -2218,15 +2218,15 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>4</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>46</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>137</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>140</v>
       </c>
@@ -2301,12 +2301,12 @@
       <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="17"/>
+    <col min="1" max="1" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="17" t="s">
         <v>110</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>95</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>96</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>97</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>98</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>99</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>100</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>101</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>102</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>103</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>104</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>105</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>106</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>107</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>108</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>109</v>
       </c>

</xml_diff>

<commit_message>
Extended ConfigEU to 44 European nations. This is useful for new users who use only Config files and want to include more non-EU countries in their models (Balkans...).
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigEU.xlsx
+++ b/ConfigFiles/ConfigEU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\svn\Dispa-SET_Public\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\Dispa_EU\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2521CA-973D-4047-AA3B-CA4992C5357F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901A0788-E958-4D60-92DC-00F1D472F403}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14304" yWindow="5796" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="171">
   <si>
     <t>Default value</t>
   </si>
@@ -493,6 +493,48 @@
   </si>
   <si>
     <t>Database/Heat_demand/2016.csv</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>MK</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>XK</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>UA</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>LI</t>
   </si>
 </sst>
 </file>
@@ -1003,24 +1045,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="B81" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="20.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="96.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>54</v>
       </c>
@@ -1032,7 +1074,7 @@
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
     </row>
-    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1042,8 +1084,8 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26" t="s">
         <v>59</v>
       </c>
@@ -1054,7 +1096,7 @@
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -1064,7 +1106,7 @@
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -1078,7 +1120,7 @@
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
     </row>
-    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1087,20 +1129,20 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
@@ -1115,7 +1157,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -1129,7 +1171,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -1143,7 +1185,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
@@ -1157,7 +1199,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>88</v>
       </c>
@@ -1168,7 +1210,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>135</v>
       </c>
@@ -1180,17 +1222,17 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="C30" s="14"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
@@ -1204,7 +1246,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
@@ -1218,7 +1260,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>47</v>
       </c>
@@ -1232,7 +1274,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>49</v>
       </c>
@@ -1243,23 +1285,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:8" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
       <c r="C45" s="14"/>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>43</v>
       </c>
@@ -1273,7 +1315,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>63</v>
       </c>
@@ -1287,7 +1329,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>129</v>
       </c>
@@ -1301,25 +1343,25 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:8" s="10" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:8" s="10" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
       <c r="C60" s="15"/>
     </row>
-    <row r="61" spans="1:8" s="8" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" s="8" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7"/>
       <c r="C61" s="14"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
@@ -1334,7 +1376,7 @@
       </c>
       <c r="H62" s="11"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>1</v>
       </c>
@@ -1351,7 +1393,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
@@ -1368,7 +1410,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>38</v>
       </c>
@@ -1382,7 +1424,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>42</v>
       </c>
@@ -1403,7 +1445,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>50</v>
       </c>
@@ -1420,7 +1462,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>93</v>
       </c>
@@ -1437,7 +1479,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>132</v>
       </c>
@@ -1454,7 +1496,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>125</v>
       </c>
@@ -1470,7 +1512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>94</v>
       </c>
@@ -1488,7 +1530,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>64</v>
       </c>
@@ -1509,7 +1551,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>65</v>
       </c>
@@ -1527,7 +1569,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>126</v>
       </c>
@@ -1545,7 +1587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>127</v>
       </c>
@@ -1563,7 +1605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>130</v>
       </c>
@@ -1577,7 +1619,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>133</v>
       </c>
@@ -1595,7 +1637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>134</v>
       </c>
@@ -1613,7 +1655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>136</v>
       </c>
@@ -1627,7 +1669,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>142</v>
       </c>
@@ -1645,7 +1687,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>143</v>
       </c>
@@ -1663,268 +1705,358 @@
         <v>400</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:8" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:8" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="1:6" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="1:6" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="9"/>
       <c r="C85" s="15"/>
     </row>
-    <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C87" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F87" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="26" t="s">
         <v>53</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>22</v>
+        <v>162</v>
       </c>
       <c r="C88" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F88" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H88" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="26"/>
       <c r="B89" s="6" t="s">
-        <v>138</v>
+        <v>22</v>
       </c>
       <c r="C89" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F89" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="26"/>
       <c r="B90" s="6" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="C90" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F90" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="26"/>
       <c r="B91" s="6" t="s">
-        <v>31</v>
+        <v>138</v>
       </c>
       <c r="C91" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F91" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="F91" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="26"/>
       <c r="B92" s="6" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C92" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F92" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="F92" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="26"/>
       <c r="B93" s="6" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="C93" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>21</v>
+        <v>158</v>
       </c>
       <c r="F93" s="5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="26"/>
       <c r="B94" s="6" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C94" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="F94" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="F94" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="26"/>
       <c r="B95" s="6" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C95" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="F95" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="26"/>
       <c r="B96" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C96" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F96" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="26"/>
       <c r="B97" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C97" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F97" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="26"/>
       <c r="B98" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C98" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F98" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="26"/>
       <c r="B99" s="6" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C99" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F99" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="26"/>
       <c r="B100" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C100" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F100" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="F100" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="26"/>
       <c r="B101" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C101" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F101" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="F101" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="26"/>
       <c r="B102" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C102" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F102" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C103" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F103" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C104" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F104" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C102" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" s="6" t="s">
+      <c r="C105" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F105" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F106" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C107" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F102" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H102" s="1" t="s">
+      <c r="F107" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H107" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C108" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F108" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="9"/>
       <c r="C109" s="15"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>2</v>
       </c>
@@ -1935,7 +2067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>77</v>
       </c>
@@ -1949,7 +2081,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>78</v>
       </c>
@@ -1963,7 +2095,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>80</v>
       </c>
@@ -1974,28 +2106,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="128" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="9"/>
       <c r="C128" s="15"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B132" s="23" t="s">
         <v>95</v>
       </c>
@@ -2003,7 +2135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B133" s="23" t="s">
         <v>96</v>
       </c>
@@ -2011,7 +2143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B134" s="23" t="s">
         <v>97</v>
       </c>
@@ -2019,7 +2151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B135" s="23" t="s">
         <v>98</v>
       </c>
@@ -2027,7 +2159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B136" s="23" t="s">
         <v>99</v>
       </c>
@@ -2035,7 +2167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B137" s="23" t="s">
         <v>100</v>
       </c>
@@ -2043,7 +2175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B138" s="23" t="s">
         <v>101</v>
       </c>
@@ -2051,7 +2183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B139" s="23" t="s">
         <v>102</v>
       </c>
@@ -2059,7 +2191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B140" s="23" t="s">
         <v>103</v>
       </c>
@@ -2067,7 +2199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B141" s="23" t="s">
         <v>104</v>
       </c>
@@ -2075,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B142" s="23" t="s">
         <v>105</v>
       </c>
@@ -2083,7 +2215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B143" s="23" t="s">
         <v>106</v>
       </c>
@@ -2091,7 +2223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B144" s="23" t="s">
         <v>107</v>
       </c>
@@ -2099,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B145" s="23" t="s">
         <v>108</v>
       </c>
@@ -2107,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B146" s="23" t="s">
         <v>109</v>
       </c>
@@ -2115,10 +2247,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F165" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B87:B108">
+    <sortCondition ref="B87"/>
+  </sortState>
   <mergeCells count="4">
     <mergeCell ref="B6:H6"/>
     <mergeCell ref="A88:A102"/>
@@ -2165,7 +2300,7 @@
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F88:G102 C88:C102 C132:C146</xm:sqref>
+          <xm:sqref>F103:F108 F87 C132:C146 F88:G102 C87:C108</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write excel files" prompt="If set to true, one excel file per parameter will be written in the simulation environment directory." xr:uid="{00000000-0002-0000-0000-000012000000}">
           <x14:formula1>
@@ -2218,15 +2353,15 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>4</v>
       </c>
@@ -2240,7 +2375,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2254,7 +2389,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2265,7 +2400,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>46</v>
       </c>
@@ -2273,7 +2408,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>137</v>
       </c>
@@ -2281,7 +2416,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>140</v>
       </c>
@@ -2301,12 +2436,12 @@
       <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="1" max="1" width="9.109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="17" t="s">
         <v>110</v>
       </c>
@@ -2350,7 +2485,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>95</v>
       </c>
@@ -2397,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>96</v>
       </c>
@@ -2444,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>97</v>
       </c>
@@ -2491,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>98</v>
       </c>
@@ -2538,7 +2673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>99</v>
       </c>
@@ -2585,7 +2720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>100</v>
       </c>
@@ -2632,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>101</v>
       </c>
@@ -2679,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>102</v>
       </c>
@@ -2726,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>103</v>
       </c>
@@ -2773,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>104</v>
       </c>
@@ -2820,7 +2955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>105</v>
       </c>
@@ -2867,7 +3002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>106</v>
       </c>
@@ -2914,7 +3049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>107</v>
       </c>
@@ -2961,7 +3096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>108</v>
       </c>
@@ -3008,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>109</v>
       </c>

</xml_diff>

<commit_message>
Minor fix for build_and_run_EU_model script (country -> zone) and ConfigEU file update
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigEU.xlsx
+++ b/ConfigFiles/ConfigEU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\Dispa_EU\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matij\Documents\Github\Dispa-SET\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901A0788-E958-4D60-92DC-00F1D472F403}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87DC4E9-8CC2-4637-B25A-741F6AB3B2E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14304" yWindow="5796" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="171">
   <si>
     <t>Default value</t>
   </si>
@@ -1045,8 +1045,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B81" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>